<commit_message>
Minor updates to data files and analyses
</commit_message>
<xml_diff>
--- a/Database/EUGCOMM_TRAITS.xlsx
+++ b/Database/EUGCOMM_TRAITS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Øystein Opedal\Dropbox\Papers\Euglossine communities\subm. files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\eugcomm\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E0973E-0696-493F-9016-E7DD3DE920D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD40F3C-7ABD-4E50-8103-7D6CC73B2165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,15 @@
     <sheet name="Variable codes" sheetId="3" r:id="rId2"/>
     <sheet name="Data sources" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1166,9 +1174,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ1057"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="P156" sqref="P156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1967,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="P29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R29">
         <v>4</v>
@@ -2069,7 +2077,7 @@
         <v>61</v>
       </c>
       <c r="P33">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="R33" s="1">
         <v>1</v>
@@ -2138,7 +2146,7 @@
         <v>2</v>
       </c>
       <c r="P36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S36" s="1">
         <v>1</v>
@@ -2183,7 +2191,7 @@
         <v>6</v>
       </c>
       <c r="P38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R38" s="1">
         <v>3</v>
@@ -2223,8 +2231,8 @@
       <c r="O39" s="3">
         <v>4</v>
       </c>
-      <c r="P39" s="3">
-        <v>1</v>
+      <c r="P39">
+        <v>2</v>
       </c>
       <c r="R39">
         <v>1</v>
@@ -2256,7 +2264,7 @@
         <v>5</v>
       </c>
       <c r="P40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S40">
         <v>1</v>
@@ -2345,7 +2353,7 @@
         <v>5</v>
       </c>
       <c r="P44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R44" s="1">
         <v>5</v>
@@ -2371,7 +2379,7 @@
         <v>71</v>
       </c>
       <c r="P45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R45">
         <v>1</v>
@@ -2435,7 +2443,7 @@
         <v>4</v>
       </c>
       <c r="P48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R48" s="1">
         <v>3</v>
@@ -2581,7 +2589,7 @@
         <v>2</v>
       </c>
       <c r="P53">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R53">
         <v>3</v>
@@ -2654,7 +2662,7 @@
         <v>1</v>
       </c>
       <c r="P55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R55" s="1">
         <v>1</v>
@@ -2715,7 +2723,7 @@
         <v>2</v>
       </c>
       <c r="P57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R57" s="1">
         <v>9</v>
@@ -2761,8 +2769,8 @@
       <c r="O58" s="1">
         <v>10</v>
       </c>
-      <c r="P58" s="3">
-        <v>10</v>
+      <c r="P58">
+        <v>14</v>
       </c>
       <c r="Q58">
         <v>1</v>
@@ -3007,7 +3015,7 @@
         <v>6</v>
       </c>
       <c r="P65">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R65">
         <v>1</v>
@@ -3164,8 +3172,8 @@
       <c r="O70">
         <v>9</v>
       </c>
-      <c r="P70" s="3">
-        <v>13</v>
+      <c r="P70">
+        <v>16</v>
       </c>
       <c r="S70">
         <v>3</v>
@@ -3200,7 +3208,7 @@
       <c r="O71">
         <v>2</v>
       </c>
-      <c r="P71" s="3">
+      <c r="P71">
         <v>3</v>
       </c>
       <c r="S71" s="1">
@@ -3418,7 +3426,7 @@
         <v>5</v>
       </c>
       <c r="P77">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="R77" s="1">
         <v>9</v>
@@ -3504,7 +3512,7 @@
         <v>5</v>
       </c>
       <c r="P79">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="R79" s="1">
         <v>13</v>
@@ -3557,7 +3565,7 @@
         <v>1</v>
       </c>
       <c r="P80">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R80">
         <v>2</v>
@@ -3582,8 +3590,8 @@
       <c r="O81" s="3">
         <v>5</v>
       </c>
-      <c r="P81" s="3">
-        <v>5</v>
+      <c r="P81">
+        <v>7</v>
       </c>
       <c r="Q81">
         <v>1</v>
@@ -3611,8 +3619,8 @@
       <c r="N82" s="3">
         <v>2</v>
       </c>
-      <c r="P82" s="3">
-        <v>4</v>
+      <c r="P82">
+        <v>5</v>
       </c>
       <c r="S82">
         <v>1</v>
@@ -3677,7 +3685,7 @@
         <v>1</v>
       </c>
       <c r="P86">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3823,7 +3831,7 @@
         <v>8</v>
       </c>
       <c r="P93">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="R93">
         <v>1</v>
@@ -3890,7 +3898,7 @@
         <v>4</v>
       </c>
       <c r="P95">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R95" s="1">
         <v>11</v>
@@ -3934,7 +3942,7 @@
         <v>2</v>
       </c>
       <c r="P96">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R96" s="1">
         <v>4</v>
@@ -3994,7 +4002,7 @@
         <v>1</v>
       </c>
       <c r="P99">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R99" s="1">
         <v>2</v>
@@ -4074,7 +4082,7 @@
         <v>4</v>
       </c>
       <c r="P103">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R103" s="1">
         <v>5</v>
@@ -4181,8 +4189,8 @@
       <c r="O109" s="3">
         <v>15</v>
       </c>
-      <c r="P109" s="3">
-        <v>13</v>
+      <c r="P109">
+        <v>16</v>
       </c>
       <c r="R109" s="3">
         <v>2</v>
@@ -4373,8 +4381,8 @@
       <c r="O117">
         <v>1</v>
       </c>
-      <c r="P117" s="3">
-        <v>5</v>
+      <c r="P117">
+        <v>7</v>
       </c>
       <c r="R117" s="1">
         <v>3</v>
@@ -4408,8 +4416,8 @@
       <c r="O118" s="3">
         <v>11</v>
       </c>
-      <c r="P118" s="3">
-        <v>12</v>
+      <c r="P118">
+        <v>15</v>
       </c>
       <c r="R118" s="1">
         <v>2</v>
@@ -4493,7 +4501,7 @@
         <v>3</v>
       </c>
       <c r="P121">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R121">
         <v>1</v>
@@ -4575,7 +4583,7 @@
         <v>12</v>
       </c>
       <c r="P123">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="R123">
         <v>1</v>
@@ -4778,7 +4786,7 @@
         <v>123</v>
       </c>
       <c r="P131">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S131">
         <v>1</v>
@@ -4911,8 +4919,8 @@
       <c r="O135" s="1">
         <v>18</v>
       </c>
-      <c r="P135" s="3">
-        <v>8</v>
+      <c r="P135">
+        <v>11</v>
       </c>
       <c r="R135" s="1">
         <v>8</v>
@@ -5069,7 +5077,7 @@
         <v>7</v>
       </c>
       <c r="P140">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R140" s="1">
         <v>14</v>
@@ -5128,7 +5136,7 @@
         <v>4</v>
       </c>
       <c r="P141">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R141" s="1">
         <v>7</v>
@@ -5174,8 +5182,8 @@
       <c r="O142" s="1">
         <v>2</v>
       </c>
-      <c r="P142" s="3">
-        <v>28</v>
+      <c r="P142">
+        <v>34</v>
       </c>
       <c r="R142" s="1">
         <v>5</v>
@@ -5291,6 +5299,9 @@
       <c r="O146" s="1">
         <v>2</v>
       </c>
+      <c r="P146">
+        <v>1</v>
+      </c>
       <c r="R146" s="1">
         <v>1</v>
       </c>
@@ -5404,7 +5415,7 @@
         <v>11</v>
       </c>
       <c r="P151">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R151" s="1">
         <v>9</v>
@@ -5436,7 +5447,7 @@
         <v>1</v>
       </c>
       <c r="P152">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R152" s="1">
         <v>2</v>
@@ -5482,8 +5493,8 @@
       <c r="O153" s="1">
         <v>19</v>
       </c>
-      <c r="P153" s="3">
-        <v>22</v>
+      <c r="P153">
+        <v>26</v>
       </c>
       <c r="R153" s="1">
         <v>11</v>
@@ -6471,7 +6482,7 @@
   <dimension ref="B1:D1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>